<commit_message>
regenerate configuration 11 + evaluation
</commit_message>
<xml_diff>
--- a/test-code-generator/Evaluation/QuantitativeEvaluation/1/UC1_TC1.xlsx
+++ b/test-code-generator/Evaluation/QuantitativeEvaluation/1/UC1_TC1.xlsx
@@ -620,11 +620,11 @@
         </is>
       </c>
       <c r="B12" s="3" t="n">
-        <v>0.240177625605921</v>
+        <v>0.2272743997994694</v>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>{'codebleu': 0.24017762560592104, 'ngram_match_score': 0.073731865886615, 'weighted_ngram_match_score': 0.09971796455614086, 'syntax_match_score': 0.47113163972286376, 'dataflow_match_score': 0.3161290322580645}</t>
+          <t>{'codebleu': 0.22727439979946942, 'ngram_match_score': 0.073731865886615, 'weighted_ngram_match_score': 0.09971796455614086, 'syntax_match_score': 0.47113163972286376, 'dataflow_match_score': 0.2645161290322581}</t>
         </is>
       </c>
       <c r="D12" s="7" t="inlineStr">

</xml_diff>